<commit_message>
Chnage the excel file to show better more accurate server requests
</commit_message>
<xml_diff>
--- a/server/Out-of-this-world.xlsx
+++ b/server/Out-of-this-world.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Софтуни\Angular\workshops\Rest-api-fan-art\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Софтуни\ReactJS\react-project\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBC1A87-67FA-4546-961B-ED0130CDBBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60FC233-53C5-4389-BF8F-8C715E883349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve"> Logging out</t>
   </si>
   <si>
-    <t xml:space="preserve"> YES</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /logout</t>
   </si>
   <si>
@@ -81,18 +78,12 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Get all fan arts</t>
-  </si>
-  <si>
     <t>user info/ Verify if user is logged in</t>
   </si>
   <si>
     <t>/users/profile</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t xml:space="preserve">PUT </t>
   </si>
   <si>
@@ -102,61 +93,106 @@
     <t xml:space="preserve"> /users/profile</t>
   </si>
   <si>
-    <t xml:space="preserve"> "username", "email"</t>
-  </si>
-  <si>
     <t>username, "email", "password", "rePassword"</t>
   </si>
   <si>
-    <t xml:space="preserve"> /fanArts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/catalog</t>
-  </si>
-  <si>
-    <t>Get a fan art</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/:fanArtId</t>
-  </si>
-  <si>
-    <t>Get my fan arts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/myFanarts</t>
-  </si>
-  <si>
-    <t>Create a fan art</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/create</t>
-  </si>
-  <si>
-    <t>Like a fan art</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/:fanArtId/like</t>
-  </si>
-  <si>
-    <t>Edit a fan art</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/:fanArtId/edit</t>
-  </si>
-  <si>
-    <t>Delete a fan art</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /fanArts/:fanArtId/delete</t>
-  </si>
-  <si>
-    <t>fanArtId</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>Get latest fan arts</t>
+    <t xml:space="preserve"> Yes</t>
+  </si>
+  <si>
+    <t>Get all movies</t>
+  </si>
+  <si>
+    <t>Get my movies</t>
+  </si>
+  <si>
+    <t>Get a movie</t>
+  </si>
+  <si>
+    <t>Create a movie</t>
+  </si>
+  <si>
+    <t>Like a movie</t>
+  </si>
+  <si>
+    <t>Edit a movie</t>
+  </si>
+  <si>
+    <t>Delete a movie</t>
+  </si>
+  <si>
+    <t>movieId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/mymovies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/create</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/:movieId/like</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/:movieId/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/:movieId/delete</t>
+  </si>
+  <si>
+    <t>Get top movies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/details/:movieId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/catalog/top</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /movies/myMovies</t>
+  </si>
+  <si>
+    <t>EDIT</t>
+  </si>
+  <si>
+    <t>"title" 'tag' 'year' 'description' 'isPublic'</t>
+  </si>
+  <si>
+    <t>movieId,  "title" 'tag' 'year' 'description' 'isPublic'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "username", "email" "image" - not-required</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /blog/comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /blog/comments/top</t>
+  </si>
+  <si>
+    <t>Get top comments</t>
+  </si>
+  <si>
+    <t>Get all comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /blog/create</t>
+  </si>
+  <si>
+    <t>Create a comment</t>
+  </si>
+  <si>
+    <t>"text",  'rating'</t>
+  </si>
+  <si>
+    <t>Delete a comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /blog/:commentId/delete</t>
   </si>
 </sst>
 </file>
@@ -316,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -367,10 +403,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -380,6 +419,117 @@
   <dxfs count="10">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -410,117 +560,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -535,14 +574,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{774E0217-B248-4902-A657-3EC42AB6ADCE}" name="Таблица1" displayName="Таблица1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:E16" xr:uid="{774E0217-B248-4902-A657-3EC42AB6ADCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{774E0217-B248-4902-A657-3EC42AB6ADCE}" name="Таблица1" displayName="Таблица1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E32" xr:uid="{774E0217-B248-4902-A657-3EC42AB6ADCE}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3EA8D5C0-7B4F-4378-BA5D-62685E5B7CF9}" name="HTTP  Method " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{06852C2F-7D1B-4832-92C0-BE0CBE363919}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E1A74521-45AF-4834-94BC-C75D45317AB1}" name=" Endpoint " dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{AA60A2BC-9532-4338-A463-8DB2B1C61B8C}" name="Expect " dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6055105E-4282-4E2B-95C2-0B473CD797E6}" name="Login Required" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3EA8D5C0-7B4F-4378-BA5D-62685E5B7CF9}" name="HTTP  Method " dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{06852C2F-7D1B-4832-92C0-BE0CBE363919}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E1A74521-45AF-4834-94BC-C75D45317AB1}" name=" Endpoint " dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AA60A2BC-9532-4338-A463-8DB2B1C61B8C}" name="Expect " dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6055105E-4282-4E2B-95C2-0B473CD797E6}" name="Login Required" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -811,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,10 +908,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -898,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -918,11 +957,11 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -936,17 +975,17 @@
     </row>
     <row r="5" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -958,21 +997,21 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="42" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1018,17 +1057,17 @@
     </row>
     <row r="9" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1042,17 +1081,17 @@
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1066,17 +1105,15 @@
     </row>
     <row r="11" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1092,19 +1129,19 @@
     </row>
     <row r="12" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1118,17 +1155,17 @@
     </row>
     <row r="13" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1140,21 +1177,21 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1168,19 +1205,19 @@
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1192,21 +1229,21 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>17</v>
+    <row r="16" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1219,11 +1256,21 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="A17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1235,11 +1282,11 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1251,11 +1298,11 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1267,11 +1314,19 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1283,11 +1338,19 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1299,11 +1362,21 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1314,40 +1387,83 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+    <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>